<commit_message>
update data template linked
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mroot\Documents\ORNL\VERIFI\src\assets\csv_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\AMO Tools\Dashboard - VERIFI\Data Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{013BDDAC-5B8C-4406-AD31-68A4594E1678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="F+1QkVH6uwlgjFH4nZhlJlf2hFPHGuSd4G1I16Xf6aaHJ+fTIM2jmGVbk5Knwl4W1k7v9JkwUx1Q9nsFZYxd/w==" workbookSaltValue="Kmj6OHG69f139UN7LGGJHQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CA2E5A-AD7F-4F13-8B77-E2226AA680CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2145" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="8" r:id="rId1"/>
     <sheet name="Meters-Utilities" sheetId="4" r:id="rId2"/>
     <sheet name="Electricity" sheetId="6" r:id="rId3"/>
     <sheet name="Non-electricity" sheetId="5" r:id="rId4"/>
-    <sheet name="HIDE" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="Predictors" sheetId="9" r:id="rId5"/>
+    <sheet name="HIDE" sheetId="7" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="ElectricityFuel">HIDE!$E$18</definedName>
@@ -29,7 +29,7 @@
     <definedName name="NaturalGasunits">HIDE!$B$52:$B$64</definedName>
     <definedName name="OtherEnergyFuel">HIDE!$D$18:$D$22</definedName>
     <definedName name="OtherEnergySLG">HIDE!$B$12</definedName>
-    <definedName name="OtherEnergyunits">HIDE!$F$52:$F$64</definedName>
+    <definedName name="OtherEnergyunits">HIDE!$F$52:$F$66</definedName>
     <definedName name="OtherFuelsGasFuel">HIDE!$A$18:$A$25</definedName>
     <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$64</definedName>
     <definedName name="OtherFuelsLiquidFuel">HIDE!$B$18:$B$48</definedName>
@@ -48,7 +48,7 @@
     <definedName name="WaterSLG">HIDE!$E$12</definedName>
     <definedName name="Waterunits">HIDE!$G$52:$G$55</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="151">
   <si>
     <t>Meter Number</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Nm3</t>
   </si>
   <si>
-    <t>MMBTu</t>
-  </si>
-  <si>
     <t>tons</t>
   </si>
   <si>
@@ -498,12 +495,36 @@
   </si>
   <si>
     <t>Sources</t>
+  </si>
+  <si>
+    <t>MMBTU</t>
+  </si>
+  <si>
+    <t>gal-F</t>
+  </si>
+  <si>
+    <t>ton-hr</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>CDD</t>
+  </si>
+  <si>
+    <t>Predictor3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -981,7 +1002,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -989,6 +1010,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1058,9 +1087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>31749</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1076,7 +1105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609599" y="361950"/>
-          <a:ext cx="12833350" cy="6362700"/>
+          <a:ext cx="12830175" cy="7210425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1127,6 +1156,15 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> template is used both for setting up an initial data upload and for updating VERIFI each month, if you choose not to enter data manually within VERIFI. When uploading, you will be able to either replace your existing data (if you changed or updated some value entered previously) or ignore existing data and only upload what is new.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>This worksheet is password protected to protect the column names.  If you need to unlock it to modify the column widths or other things to better match your facility, the password is "VERIFI" but PLEASE do not change the column names (with the exception of the Predictors tab) as that will break VERIFI's ability to import data from this template.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
@@ -1308,6 +1346,21 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>This tab is where you enter data for any other utility you wish to track, just be sure to have the correct meter number for each row.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Predictors</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>This tab is where you enter data pertaining to any predictors for correlation or regression analysis (weather data, production data, etc.).  On this tab, you can change the column names to match your facility (with the exception of "Date")</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1617,12 +1670,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
-  <sheetProtection algorithmName="SHA-512" hashValue="/c7y3BBb3XiGNjaKmFRJfTDF6/chhUwTa7Oh1PZqSr+4BhvqBbdJJx0jLnvsu0/AwUCbEcFJ9XVmfyM9Bq+kuA==" saltValue="szmZa2/IpY7/dYhmqqccUA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+j/LUuc75Pyo4KzhrpkVGkDcHNvi1nbJnEAlC4kMemcZ4tbRn5pO3xJgrg3+MWoAZV2qA60pRHKcQFSsBtTU0w==" saltValue="us7YpYgy6P2SfZ7DAZ5chA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1633,24 +1686,25 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="12.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1746,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HewrPq+G7xrREWgahqw4KECRmWlduqN5/uU7r221AsqekTWwYjtzfl1l2yrfAXZqEsS8qTrKjh9MC6vn8wpMnA==" saltValue="/GnEKEmrBd6fASME4aPqyg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Oa6FUWb1LNh4fqGDLKRbjgvJ0DR6K726XiWg5i9vEKr2P+0Hj+hSJ2mG/U+yokCfIcMkZ2oHMc04lWhsNdFSvQ==" saltValue="O04A5Gke2Qf8tjb54319mQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Sources</formula1>
@@ -1716,28 +1770,28 @@
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" style="4" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16" width="11.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="1" customWidth="1"/>
-    <col min="20" max="24" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="1" customWidth="1"/>
+    <col min="6" max="16" width="11.1796875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.54296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.08984375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7265625" style="1" customWidth="1"/>
+    <col min="20" max="24" width="11.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1808,8 +1862,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FKeZb/tRedkDauLxn5RJf8qZQXRzMIxQ7SO36qcoxUIpiHA9iInYkIYwvMc+1r+y6Son++dY6lS5OI6jppljXQ==" saltValue="Rp6wAACEr7FqlW+SR2rxiw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dANAtv2Wkc6L0I7KV6MvSh6WAFQBkjKJUZOIG64VLnlVTPL7cWMjakdwWEp4UEePUC8lqCtgY28x7q+k3zyg7A==" saltValue="wufavQG4Wd8gSLrPO+k7zg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1818,23 +1873,25 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.08984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
@@ -1854,383 +1911,420 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="x4/ocRpciuzXg72nUcMQZcRUBZX1RQsvR7pdcjhJJE8J1rf/W5ks/d5MarxIl3z+V1sGSHKCz8qgQOMpTeRGkA==" saltValue="G/JWaDdVBS7iw9Dsyri/HA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="gi0ackw9LJ66nLQXDN6fzBMg+QTmhbCUyrmAgzUiwyoC0ka/ipjq8eMwMcGO62n+NR75KT/iTlmU+DuAWjg7rA==" saltValue="RD7/ZZYvJj7xJue/opeydw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C580699A-D75E-4771-B742-42694586E774}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="10.08984375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="hEJYitYbSasUc4EEmNj0+GQijzQul14A7pc8Q42BRwdqD0EgakX8CNyNZFCGaUmN/u2E9upTwi19RydZ/7PGEw==" saltValue="vyout2A3FD2Se4iyhQgg7A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
         <v>119</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>120</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>121</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>122</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>123</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>124</v>
       </c>
-      <c r="G11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
         <v>135</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>136</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>137</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>138</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>139</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>140</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>141</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>142</v>
       </c>
-      <c r="I17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>72</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>68</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
         <v>96</v>
       </c>
-      <c r="B21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>98</v>
       </c>
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" t="s">
         <v>130</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" t="s">
         <v>131</v>
       </c>
-      <c r="C51" t="s">
-        <v>126</v>
-      </c>
-      <c r="D51" t="s">
-        <v>127</v>
-      </c>
-      <c r="E51" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" t="s">
-        <v>129</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>132</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>133</v>
       </c>
-      <c r="I51" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2259,7 +2353,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2288,165 +2382,165 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="F54" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="G54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G55" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>62</v>
       </c>
-      <c r="H55" t="s">
+      <c r="B56" t="s">
         <v>62</v>
       </c>
-      <c r="I55" t="s">
+      <c r="C56" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="D56" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56" t="s">
+        <v>62</v>
+      </c>
+      <c r="F56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>63</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>63</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>63</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>63</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>63</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>64</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>64</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>64</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>64</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>64</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>65</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>65</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>65</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>65</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>65</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>66</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>66</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>66</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>66</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>66</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" t="s">
-        <v>67</v>
-      </c>
-      <c r="C60" t="s">
-        <v>67</v>
-      </c>
-      <c r="D60" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" t="s">
-        <v>67</v>
-      </c>
-      <c r="F60" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -2463,7 +2557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>55</v>
       </c>
@@ -2480,24 +2574,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>51</v>
       </c>
@@ -2505,13 +2599,23 @@
         <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F64" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F65" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F66" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated import template and fix broken link with relative path
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\AMO Tools\Dashboard - VERIFI\Data Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CA2E5A-AD7F-4F13-8B77-E2226AA680CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED13D9-3C07-4DBD-9F85-E8983DDC5B11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2145" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <definedName name="WaterSLG">HIDE!$E$12</definedName>
     <definedName name="Waterunits">HIDE!$G$52:$G$55</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -497,9 +497,6 @@
     <t>Sources</t>
   </si>
   <si>
-    <t>MMBTU</t>
-  </si>
-  <si>
     <t>gal-F</t>
   </si>
   <si>
@@ -516,6 +513,9 @@
   </si>
   <si>
     <t>Predictor3</t>
+  </si>
+  <si>
+    <t>MMBtu</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1010,14 +1010,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1670,7 +1670,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1935,16 +1935,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1959,7 +1959,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2384,22 +2384,22 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F54" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G54" t="s">
         <v>57</v>
@@ -2610,12 +2610,12 @@
     </row>
     <row r="65" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F66" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template and add MCF gas unit
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\AMO Tools\Dashboard - VERIFI\Data Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mroot\Documents\ORNL\VERIFI\src\assets\csv_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED13D9-3C07-4DBD-9F85-E8983DDC5B11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47C6007D-AEAD-469E-8144-26B95A7BD993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2145" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="8" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <definedName name="Electricityunits">HIDE!$A$52:$A$60</definedName>
     <definedName name="NaturalGasFuel">HIDE!$F$18</definedName>
     <definedName name="NaturalGasSLG">HIDE!$D$12</definedName>
-    <definedName name="NaturalGasunits">HIDE!$B$52:$B$64</definedName>
+    <definedName name="NaturalGasunits">HIDE!$B$52:$B$65</definedName>
     <definedName name="OtherEnergyFuel">HIDE!$D$18:$D$22</definedName>
     <definedName name="OtherEnergySLG">HIDE!$B$12</definedName>
     <definedName name="OtherEnergyunits">HIDE!$F$52:$F$66</definedName>
     <definedName name="OtherFuelsGasFuel">HIDE!$A$18:$A$25</definedName>
-    <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$64</definedName>
+    <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$65</definedName>
     <definedName name="OtherFuelsLiquidFuel">HIDE!$B$18:$B$48</definedName>
     <definedName name="OtherFuelsLiquidunits">HIDE!$D$52:$D$64</definedName>
     <definedName name="OtherFuelsSLG">HIDE!$A$12:$A$14</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="152">
   <si>
     <t>Meter Number</t>
   </si>
@@ -516,6 +516,9 @@
   </si>
   <si>
     <t>MMBtu</t>
+  </si>
+  <si>
+    <t>MCF</t>
   </si>
 </sst>
 </file>
@@ -1669,15 +1672,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE50A05-F3FD-4276-B756-550777F28C99}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="+j/LUuc75Pyo4KzhrpkVGkDcHNvi1nbJnEAlC4kMemcZ4tbRn5pO3xJgrg3+MWoAZV2qA60pRHKcQFSsBtTU0w==" saltValue="us7YpYgy6P2SfZ7DAZ5chA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1685,26 +1689,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="12.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="33.6328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.36328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1762,6 +1766,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1773,21 +1778,21 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="1" customWidth="1"/>
-    <col min="6" max="16" width="11.1796875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.54296875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.08984375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7265625" style="1" customWidth="1"/>
-    <col min="20" max="24" width="11.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16" width="11.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="1" customWidth="1"/>
+    <col min="20" max="24" width="11.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1876,18 +1881,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1925,15 +1930,15 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
-    <col min="2" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="10.08984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="4"/>
+    <col min="2" max="3" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>146</v>
       </c>
@@ -1958,53 +1963,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -2027,22 +2032,22 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -2071,7 +2076,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2099,7 +2104,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -2113,7 +2118,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -2127,7 +2132,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -2141,7 +2146,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -2152,7 +2157,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -2163,7 +2168,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -2174,7 +2179,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>84</v>
       </c>
@@ -2182,7 +2187,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>85</v>
       </c>
@@ -2190,112 +2195,112 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -2324,7 +2329,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2353,7 +2358,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2382,7 +2387,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>150</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2460,7 +2465,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2480,7 +2485,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2500,7 +2505,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2520,7 +2525,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2540,7 +2545,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -2557,7 +2562,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>55</v>
       </c>
@@ -2574,7 +2579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>58</v>
       </c>
@@ -2591,7 +2596,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>51</v>
       </c>
@@ -2608,12 +2613,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" t="s">
+        <v>151</v>
+      </c>
       <c r="F65" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
Revert "Update Master v0.4.0-alpha"
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mroot\Documents\ORNL\VERIFI\src\assets\csv_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\AMO Tools\Dashboard - VERIFI\Data Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47C6007D-AEAD-469E-8144-26B95A7BD993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED13D9-3C07-4DBD-9F85-E8983DDC5B11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2145" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="8" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <definedName name="Electricityunits">HIDE!$A$52:$A$60</definedName>
     <definedName name="NaturalGasFuel">HIDE!$F$18</definedName>
     <definedName name="NaturalGasSLG">HIDE!$D$12</definedName>
-    <definedName name="NaturalGasunits">HIDE!$B$52:$B$65</definedName>
+    <definedName name="NaturalGasunits">HIDE!$B$52:$B$64</definedName>
     <definedName name="OtherEnergyFuel">HIDE!$D$18:$D$22</definedName>
     <definedName name="OtherEnergySLG">HIDE!$B$12</definedName>
     <definedName name="OtherEnergyunits">HIDE!$F$52:$F$66</definedName>
     <definedName name="OtherFuelsGasFuel">HIDE!$A$18:$A$25</definedName>
-    <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$65</definedName>
+    <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$64</definedName>
     <definedName name="OtherFuelsLiquidFuel">HIDE!$B$18:$B$48</definedName>
     <definedName name="OtherFuelsLiquidunits">HIDE!$D$52:$D$64</definedName>
     <definedName name="OtherFuelsSLG">HIDE!$A$12:$A$14</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="151">
   <si>
     <t>Meter Number</t>
   </si>
@@ -516,9 +516,6 @@
   </si>
   <si>
     <t>MMBtu</t>
-  </si>
-  <si>
-    <t>MCF</t>
   </si>
 </sst>
 </file>
@@ -1672,16 +1669,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE50A05-F3FD-4276-B756-550777F28C99}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="+j/LUuc75Pyo4KzhrpkVGkDcHNvi1nbJnEAlC4kMemcZ4tbRn5pO3xJgrg3+MWoAZV2qA60pRHKcQFSsBtTU0w==" saltValue="us7YpYgy6P2SfZ7DAZ5chA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1689,26 +1685,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="12.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1762,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1778,21 +1773,21 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" style="4" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16" width="11.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="1" customWidth="1"/>
-    <col min="20" max="24" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="1" customWidth="1"/>
+    <col min="6" max="16" width="11.1796875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.54296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.08984375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7265625" style="1" customWidth="1"/>
+    <col min="20" max="24" width="11.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1881,18 +1876,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.08984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1930,15 +1925,15 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="4"/>
-    <col min="2" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="10.08984375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>146</v>
       </c>
@@ -1963,53 +1958,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -2032,22 +2027,22 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -2076,7 +2071,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2090,7 +2085,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2104,7 +2099,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -2118,7 +2113,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -2132,7 +2127,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -2146,7 +2141,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -2157,7 +2152,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -2168,7 +2163,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -2179,7 +2174,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>84</v>
       </c>
@@ -2187,7 +2182,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>85</v>
       </c>
@@ -2195,112 +2190,112 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -2329,7 +2324,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2358,7 +2353,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2387,7 +2382,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>150</v>
       </c>
@@ -2416,7 +2411,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2445,7 +2440,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2465,7 +2460,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2485,7 +2480,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2505,7 +2500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2525,7 +2520,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2545,7 +2540,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -2562,7 +2557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>55</v>
       </c>
@@ -2579,7 +2574,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>58</v>
       </c>
@@ -2596,7 +2591,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>51</v>
       </c>
@@ -2613,18 +2608,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>151</v>
-      </c>
-      <c r="C65" t="s">
-        <v>151</v>
-      </c>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F65" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F66" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Update Master v0.4.0-alpha""
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\AMO Tools\Dashboard - VERIFI\Data Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mroot\Documents\ORNL\VERIFI\src\assets\csv_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED13D9-3C07-4DBD-9F85-E8983DDC5B11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47C6007D-AEAD-469E-8144-26B95A7BD993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2145" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="8" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <definedName name="Electricityunits">HIDE!$A$52:$A$60</definedName>
     <definedName name="NaturalGasFuel">HIDE!$F$18</definedName>
     <definedName name="NaturalGasSLG">HIDE!$D$12</definedName>
-    <definedName name="NaturalGasunits">HIDE!$B$52:$B$64</definedName>
+    <definedName name="NaturalGasunits">HIDE!$B$52:$B$65</definedName>
     <definedName name="OtherEnergyFuel">HIDE!$D$18:$D$22</definedName>
     <definedName name="OtherEnergySLG">HIDE!$B$12</definedName>
     <definedName name="OtherEnergyunits">HIDE!$F$52:$F$66</definedName>
     <definedName name="OtherFuelsGasFuel">HIDE!$A$18:$A$25</definedName>
-    <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$64</definedName>
+    <definedName name="OtherFuelsGasunits">HIDE!$C$52:$C$65</definedName>
     <definedName name="OtherFuelsLiquidFuel">HIDE!$B$18:$B$48</definedName>
     <definedName name="OtherFuelsLiquidunits">HIDE!$D$52:$D$64</definedName>
     <definedName name="OtherFuelsSLG">HIDE!$A$12:$A$14</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="152">
   <si>
     <t>Meter Number</t>
   </si>
@@ -516,6 +516,9 @@
   </si>
   <si>
     <t>MMBtu</t>
+  </si>
+  <si>
+    <t>MCF</t>
   </si>
 </sst>
 </file>
@@ -1669,15 +1672,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE50A05-F3FD-4276-B756-550777F28C99}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="+j/LUuc75Pyo4KzhrpkVGkDcHNvi1nbJnEAlC4kMemcZ4tbRn5pO3xJgrg3+MWoAZV2qA60pRHKcQFSsBtTU0w==" saltValue="us7YpYgy6P2SfZ7DAZ5chA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1685,26 +1689,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="12.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="33.6328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.36328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1762,6 +1766,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1773,21 +1778,21 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="1" customWidth="1"/>
-    <col min="6" max="16" width="11.1796875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.54296875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.08984375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7265625" style="1" customWidth="1"/>
-    <col min="20" max="24" width="11.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16" width="11.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="1" customWidth="1"/>
+    <col min="20" max="24" width="11.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1876,18 +1881,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1925,15 +1930,15 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
-    <col min="2" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="10.08984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="4"/>
+    <col min="2" max="3" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>146</v>
       </c>
@@ -1958,53 +1963,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -2027,22 +2032,22 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -2071,7 +2076,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2099,7 +2104,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -2113,7 +2118,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -2127,7 +2132,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -2141,7 +2146,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -2152,7 +2157,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -2163,7 +2168,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -2174,7 +2179,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>84</v>
       </c>
@@ -2182,7 +2187,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>85</v>
       </c>
@@ -2190,112 +2195,112 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -2324,7 +2329,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2353,7 +2358,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2382,7 +2387,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>150</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2460,7 +2465,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2480,7 +2485,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2500,7 +2505,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2520,7 +2525,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2540,7 +2545,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -2557,7 +2562,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>55</v>
       </c>
@@ -2574,7 +2579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>58</v>
       </c>
@@ -2591,7 +2596,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>51</v>
       </c>
@@ -2608,12 +2613,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" t="s">
+        <v>151</v>
+      </c>
       <c r="F65" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
updated template with zipcode
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\Armstrong Work\DOE VERIFI\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E860086-20C7-44C9-9CB8-C0FE45282CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A63F380-3D14-4C3F-9355-5EE12EE0B0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="-21750" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="8" r:id="rId1"/>
@@ -2532,7 +2532,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2565,6 +2565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3387,7 +3388,7 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3446,7 +3447,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="6"/>
@@ -3459,7 +3460,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="6"/>
@@ -3472,7 +3473,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="6"/>
@@ -3485,7 +3486,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="6"/>
@@ -3498,7 +3499,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="6"/>
@@ -3511,7 +3512,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="6"/>
@@ -3524,7 +3525,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="14"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="6"/>
@@ -3537,7 +3538,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="6"/>
@@ -3550,7 +3551,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="6"/>
@@ -3563,7 +3564,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6"/>
@@ -3576,7 +3577,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="6"/>
@@ -3589,7 +3590,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="6"/>
@@ -3602,7 +3603,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="6"/>
@@ -3615,7 +3616,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="6"/>
@@ -3628,7 +3629,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="6"/>
@@ -3641,7 +3642,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="6"/>
@@ -3654,7 +3655,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="6"/>
@@ -3667,7 +3668,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="6"/>
@@ -3680,7 +3681,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="6"/>
@@ -3693,7 +3694,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="6"/>
@@ -3706,7 +3707,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="6"/>
@@ -3719,7 +3720,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="6"/>
@@ -3732,7 +3733,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="6"/>
@@ -3745,7 +3746,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="6"/>
@@ -3758,7 +3759,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="6"/>
@@ -3771,7 +3772,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="6"/>
@@ -3784,7 +3785,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="6"/>
@@ -3797,7 +3798,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="6"/>
@@ -3810,7 +3811,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="6"/>
@@ -3823,7 +3824,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="6"/>
@@ -3836,7 +3837,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="6"/>
@@ -3849,7 +3850,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="F33" s="14"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="6"/>
@@ -3862,7 +3863,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="F34" s="14"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="6"/>
@@ -3875,7 +3876,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+      <c r="F35" s="14"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="6"/>
@@ -3888,7 +3889,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+      <c r="F36" s="14"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="6"/>
@@ -3901,7 +3902,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="6"/>
@@ -3914,7 +3915,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="F38" s="14"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="6"/>
@@ -3927,7 +3928,7 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="6"/>
@@ -3940,7 +3941,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="6"/>
@@ -3953,7 +3954,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="F41" s="14"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="6"/>
@@ -3966,7 +3967,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="F42" s="14"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="6"/>
@@ -3979,7 +3980,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+      <c r="F43" s="14"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="6"/>
@@ -3992,7 +3993,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+      <c r="F44" s="14"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="6"/>
@@ -4005,7 +4006,7 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="F45" s="14"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="6"/>
@@ -4018,7 +4019,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
+      <c r="F46" s="14"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="6"/>
@@ -4031,7 +4032,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="F47" s="14"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="6"/>
@@ -4044,7 +4045,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="F48" s="14"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="6"/>
@@ -4057,7 +4058,7 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="F49" s="14"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="6"/>
@@ -4070,7 +4071,7 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="F50" s="14"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="6"/>
@@ -4083,7 +4084,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
+      <c r="F51" s="14"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="6"/>
@@ -4096,7 +4097,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+      <c r="F52" s="14"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="6"/>
@@ -4109,7 +4110,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="F53" s="14"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="6"/>
@@ -4122,7 +4123,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="F54" s="14"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="6"/>
@@ -4135,7 +4136,7 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="F55" s="14"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="6"/>
@@ -4148,7 +4149,7 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="F56" s="14"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="6"/>
@@ -4161,7 +4162,7 @@
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="F57" s="14"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="6"/>
@@ -4174,7 +4175,7 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="F58" s="14"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="6"/>
@@ -4187,7 +4188,7 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
+      <c r="F59" s="14"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="6"/>
@@ -4200,7 +4201,7 @@
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="F60" s="14"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="6"/>
@@ -4213,7 +4214,7 @@
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="F61" s="14"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="6"/>
@@ -4226,7 +4227,7 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="6"/>
@@ -4239,7 +4240,7 @@
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="F63" s="14"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="6"/>
@@ -4252,7 +4253,7 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
+      <c r="F64" s="14"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="6"/>
@@ -4265,7 +4266,7 @@
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
+      <c r="F65" s="14"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="6"/>
@@ -4278,7 +4279,7 @@
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="F66" s="14"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="6"/>
@@ -4291,7 +4292,7 @@
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="F67" s="14"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="6"/>
@@ -4304,7 +4305,7 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
+      <c r="F68" s="14"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="6"/>
@@ -4317,7 +4318,7 @@
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
+      <c r="F69" s="14"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="6"/>
@@ -4330,7 +4331,7 @@
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+      <c r="F70" s="14"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="6"/>
@@ -4343,7 +4344,7 @@
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
+      <c r="F71" s="14"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="6"/>
@@ -4356,7 +4357,7 @@
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
+      <c r="F72" s="14"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="6"/>
@@ -4369,7 +4370,7 @@
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
+      <c r="F73" s="14"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="6"/>
@@ -4382,7 +4383,7 @@
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
+      <c r="F74" s="14"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="6"/>
@@ -4395,7 +4396,7 @@
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
+      <c r="F75" s="14"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="6"/>
@@ -4408,7 +4409,7 @@
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
+      <c r="F76" s="14"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="6"/>
@@ -4421,7 +4422,7 @@
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
+      <c r="F77" s="14"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="6"/>
@@ -4434,7 +4435,7 @@
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
+      <c r="F78" s="14"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="6"/>
@@ -4447,7 +4448,7 @@
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="6"/>
@@ -4460,7 +4461,7 @@
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
+      <c r="F80" s="14"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="6"/>
@@ -4473,7 +4474,7 @@
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
+      <c r="F81" s="14"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="6"/>
@@ -4486,7 +4487,7 @@
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
+      <c r="F82" s="14"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="6"/>
@@ -4499,7 +4500,7 @@
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="6"/>
@@ -4512,7 +4513,7 @@
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="6"/>
@@ -4525,7 +4526,7 @@
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
+      <c r="F85" s="14"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="6"/>
@@ -4538,7 +4539,7 @@
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
+      <c r="F86" s="14"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="6"/>
@@ -4551,7 +4552,7 @@
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
+      <c r="F87" s="14"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="6"/>
@@ -4564,7 +4565,7 @@
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
+      <c r="F88" s="14"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="6"/>
@@ -4577,7 +4578,7 @@
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
+      <c r="F89" s="14"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="6"/>
@@ -4590,7 +4591,7 @@
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
+      <c r="F90" s="14"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="6"/>
@@ -4603,7 +4604,7 @@
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
+      <c r="F91" s="14"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="6"/>
@@ -4616,7 +4617,7 @@
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
+      <c r="F92" s="14"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="6"/>
@@ -4629,7 +4630,7 @@
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
+      <c r="F93" s="14"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="6"/>
@@ -4642,7 +4643,7 @@
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
+      <c r="F94" s="14"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="6"/>
@@ -4655,7 +4656,7 @@
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="6"/>
-      <c r="F95" s="6"/>
+      <c r="F95" s="14"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="6"/>
@@ -4668,7 +4669,7 @@
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
+      <c r="F96" s="14"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="6"/>
@@ -4681,7 +4682,7 @@
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="6"/>
-      <c r="F97" s="6"/>
+      <c r="F97" s="14"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="6"/>
@@ -4694,7 +4695,7 @@
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="6"/>
-      <c r="F98" s="6"/>
+      <c r="F98" s="14"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="6"/>
@@ -4707,7 +4708,7 @@
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
+      <c r="F99" s="14"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="6"/>
@@ -4720,7 +4721,7 @@
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
+      <c r="F100" s="14"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="6"/>
@@ -4733,7 +4734,7 @@
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
+      <c r="F101" s="14"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="6"/>
@@ -4746,7 +4747,7 @@
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
+      <c r="F102" s="14"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="6"/>
@@ -4759,7 +4760,7 @@
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
+      <c r="F103" s="14"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="6"/>
@@ -4772,7 +4773,7 @@
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
+      <c r="F104" s="14"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="6"/>
@@ -4785,7 +4786,7 @@
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
+      <c r="F105" s="14"/>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="6"/>
@@ -4798,7 +4799,7 @@
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
+      <c r="F106" s="14"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="6"/>
@@ -4811,7 +4812,7 @@
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="6"/>
-      <c r="F107" s="6"/>
+      <c r="F107" s="14"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="6"/>
@@ -4824,7 +4825,7 @@
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="6"/>
-      <c r="F108" s="6"/>
+      <c r="F108" s="14"/>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="6"/>
@@ -4837,7 +4838,7 @@
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
+      <c r="F109" s="14"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="6"/>
@@ -4850,7 +4851,7 @@
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="6"/>
-      <c r="F110" s="6"/>
+      <c r="F110" s="14"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="6"/>
@@ -4863,7 +4864,7 @@
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="6"/>
-      <c r="F111" s="6"/>
+      <c r="F111" s="14"/>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="6"/>
@@ -4876,7 +4877,7 @@
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="6"/>
-      <c r="F112" s="6"/>
+      <c r="F112" s="14"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="6"/>
@@ -4889,7 +4890,7 @@
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="6"/>
-      <c r="F113" s="6"/>
+      <c r="F113" s="14"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="6"/>
@@ -4902,7 +4903,7 @@
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="6"/>
-      <c r="F114" s="6"/>
+      <c r="F114" s="14"/>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="6"/>
@@ -4915,7 +4916,7 @@
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="6"/>
-      <c r="F115" s="6"/>
+      <c r="F115" s="14"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="6"/>
@@ -4928,7 +4929,7 @@
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="6"/>
-      <c r="F116" s="6"/>
+      <c r="F116" s="14"/>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="6"/>
@@ -4941,7 +4942,7 @@
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="6"/>
-      <c r="F117" s="6"/>
+      <c r="F117" s="14"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
       <c r="I117" s="6"/>
@@ -4954,7 +4955,7 @@
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="6"/>
-      <c r="F118" s="6"/>
+      <c r="F118" s="14"/>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="6"/>
@@ -4967,7 +4968,7 @@
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="6"/>
-      <c r="F119" s="6"/>
+      <c r="F119" s="14"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="6"/>
@@ -4980,7 +4981,7 @@
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
+      <c r="F120" s="14"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="6"/>
@@ -4993,7 +4994,7 @@
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
+      <c r="F121" s="14"/>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="6"/>
@@ -5006,7 +5007,7 @@
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
+      <c r="F122" s="14"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="6"/>
@@ -5019,7 +5020,7 @@
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="6"/>
-      <c r="F123" s="6"/>
+      <c r="F123" s="14"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="6"/>
@@ -5032,7 +5033,7 @@
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="6"/>
-      <c r="F124" s="6"/>
+      <c r="F124" s="14"/>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="6"/>
@@ -5045,7 +5046,7 @@
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="6"/>
-      <c r="F125" s="6"/>
+      <c r="F125" s="14"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="6"/>
@@ -5058,7 +5059,7 @@
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
+      <c r="F126" s="14"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="6"/>
@@ -5071,7 +5072,7 @@
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
       <c r="E127" s="6"/>
-      <c r="F127" s="6"/>
+      <c r="F127" s="14"/>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="6"/>
@@ -5084,7 +5085,7 @@
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
       <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
+      <c r="F128" s="14"/>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="6"/>
@@ -5097,7 +5098,7 @@
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
+      <c r="F129" s="14"/>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="6"/>
@@ -5110,7 +5111,7 @@
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
       <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
+      <c r="F130" s="14"/>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="6"/>
@@ -5123,7 +5124,7 @@
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
       <c r="E131" s="6"/>
-      <c r="F131" s="6"/>
+      <c r="F131" s="14"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="6"/>
@@ -5136,7 +5137,7 @@
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="6"/>
-      <c r="F132" s="6"/>
+      <c r="F132" s="14"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="6"/>
@@ -5149,7 +5150,7 @@
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="6"/>
-      <c r="F133" s="6"/>
+      <c r="F133" s="14"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="6"/>
@@ -5162,7 +5163,7 @@
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="6"/>
-      <c r="F134" s="6"/>
+      <c r="F134" s="14"/>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="6"/>
@@ -5175,7 +5176,7 @@
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
       <c r="E135" s="6"/>
-      <c r="F135" s="6"/>
+      <c r="F135" s="14"/>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="6"/>
@@ -5188,7 +5189,7 @@
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="6"/>
-      <c r="F136" s="6"/>
+      <c r="F136" s="14"/>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="6"/>
@@ -5201,7 +5202,7 @@
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
       <c r="E137" s="6"/>
-      <c r="F137" s="6"/>
+      <c r="F137" s="14"/>
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="6"/>
@@ -5214,7 +5215,7 @@
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="6"/>
-      <c r="F138" s="6"/>
+      <c r="F138" s="14"/>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="6"/>
@@ -5227,7 +5228,7 @@
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="6"/>
-      <c r="F139" s="6"/>
+      <c r="F139" s="14"/>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
       <c r="I139" s="6"/>
@@ -5240,7 +5241,7 @@
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="6"/>
-      <c r="F140" s="6"/>
+      <c r="F140" s="14"/>
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
       <c r="I140" s="6"/>
@@ -5253,7 +5254,7 @@
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="6"/>
-      <c r="F141" s="6"/>
+      <c r="F141" s="14"/>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
       <c r="I141" s="6"/>
@@ -5266,7 +5267,7 @@
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="6"/>
-      <c r="F142" s="6"/>
+      <c r="F142" s="14"/>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
       <c r="I142" s="6"/>
@@ -5279,7 +5280,7 @@
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
+      <c r="F143" s="14"/>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
       <c r="I143" s="6"/>
@@ -5292,7 +5293,7 @@
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
+      <c r="F144" s="14"/>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
       <c r="I144" s="6"/>
@@ -5305,7 +5306,7 @@
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="6"/>
-      <c r="F145" s="6"/>
+      <c r="F145" s="14"/>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
       <c r="I145" s="6"/>
@@ -5318,7 +5319,7 @@
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="6"/>
-      <c r="F146" s="6"/>
+      <c r="F146" s="14"/>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
       <c r="I146" s="6"/>
@@ -5331,7 +5332,7 @@
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="6"/>
-      <c r="F147" s="6"/>
+      <c r="F147" s="14"/>
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
       <c r="I147" s="6"/>
@@ -5344,7 +5345,7 @@
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="6"/>
-      <c r="F148" s="6"/>
+      <c r="F148" s="14"/>
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
       <c r="I148" s="6"/>
@@ -5357,7 +5358,7 @@
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="6"/>
-      <c r="F149" s="6"/>
+      <c r="F149" s="14"/>
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
       <c r="I149" s="6"/>
@@ -5370,7 +5371,7 @@
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="6"/>
-      <c r="F150" s="6"/>
+      <c r="F150" s="14"/>
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
       <c r="I150" s="6"/>
@@ -5383,7 +5384,7 @@
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="6"/>
-      <c r="F151" s="6"/>
+      <c r="F151" s="14"/>
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
       <c r="I151" s="6"/>
@@ -5396,7 +5397,7 @@
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="6"/>
-      <c r="F152" s="6"/>
+      <c r="F152" s="14"/>
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
       <c r="I152" s="6"/>
@@ -5409,7 +5410,7 @@
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="6"/>
-      <c r="F153" s="6"/>
+      <c r="F153" s="14"/>
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
       <c r="I153" s="6"/>
@@ -5422,7 +5423,7 @@
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="6"/>
-      <c r="F154" s="6"/>
+      <c r="F154" s="14"/>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
       <c r="I154" s="6"/>
@@ -5435,7 +5436,7 @@
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="6"/>
-      <c r="F155" s="6"/>
+      <c r="F155" s="14"/>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
       <c r="I155" s="6"/>
@@ -5448,7 +5449,7 @@
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="6"/>
-      <c r="F156" s="6"/>
+      <c r="F156" s="14"/>
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
       <c r="I156" s="6"/>
@@ -5461,7 +5462,7 @@
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="6"/>
-      <c r="F157" s="6"/>
+      <c r="F157" s="14"/>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
       <c r="I157" s="6"/>
@@ -5474,7 +5475,7 @@
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="6"/>
-      <c r="F158" s="6"/>
+      <c r="F158" s="14"/>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
       <c r="I158" s="6"/>
@@ -5487,7 +5488,7 @@
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="6"/>
-      <c r="F159" s="6"/>
+      <c r="F159" s="14"/>
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
       <c r="I159" s="6"/>
@@ -5500,7 +5501,7 @@
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="6"/>
-      <c r="F160" s="6"/>
+      <c r="F160" s="14"/>
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
       <c r="I160" s="6"/>
@@ -5513,7 +5514,7 @@
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="6"/>
-      <c r="F161" s="6"/>
+      <c r="F161" s="14"/>
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
       <c r="I161" s="6"/>
@@ -5526,7 +5527,7 @@
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="6"/>
-      <c r="F162" s="6"/>
+      <c r="F162" s="14"/>
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
       <c r="I162" s="6"/>
@@ -5539,7 +5540,7 @@
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="6"/>
-      <c r="F163" s="6"/>
+      <c r="F163" s="14"/>
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
       <c r="I163" s="6"/>
@@ -5552,7 +5553,7 @@
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
       <c r="E164" s="6"/>
-      <c r="F164" s="6"/>
+      <c r="F164" s="14"/>
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
       <c r="I164" s="6"/>
@@ -5565,7 +5566,7 @@
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
       <c r="E165" s="6"/>
-      <c r="F165" s="6"/>
+      <c r="F165" s="14"/>
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
       <c r="I165" s="6"/>
@@ -5578,7 +5579,7 @@
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="6"/>
-      <c r="F166" s="6"/>
+      <c r="F166" s="14"/>
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
       <c r="I166" s="6"/>
@@ -5591,7 +5592,7 @@
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
       <c r="E167" s="6"/>
-      <c r="F167" s="6"/>
+      <c r="F167" s="14"/>
       <c r="G167" s="3"/>
       <c r="H167" s="3"/>
       <c r="I167" s="6"/>
@@ -5604,7 +5605,7 @@
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="6"/>
-      <c r="F168" s="6"/>
+      <c r="F168" s="14"/>
       <c r="G168" s="3"/>
       <c r="H168" s="3"/>
       <c r="I168" s="6"/>
@@ -5617,7 +5618,7 @@
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="6"/>
-      <c r="F169" s="6"/>
+      <c r="F169" s="14"/>
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
       <c r="I169" s="6"/>
@@ -5630,7 +5631,7 @@
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="6"/>
-      <c r="F170" s="6"/>
+      <c r="F170" s="14"/>
       <c r="G170" s="3"/>
       <c r="H170" s="3"/>
       <c r="I170" s="6"/>
@@ -5643,7 +5644,7 @@
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="6"/>
-      <c r="F171" s="6"/>
+      <c r="F171" s="14"/>
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
       <c r="I171" s="6"/>
@@ -5656,7 +5657,7 @@
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="6"/>
-      <c r="F172" s="6"/>
+      <c r="F172" s="14"/>
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
       <c r="I172" s="6"/>
@@ -5669,7 +5670,7 @@
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
       <c r="E173" s="6"/>
-      <c r="F173" s="6"/>
+      <c r="F173" s="14"/>
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
       <c r="I173" s="6"/>
@@ -5682,7 +5683,7 @@
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="6"/>
-      <c r="F174" s="6"/>
+      <c r="F174" s="14"/>
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
       <c r="I174" s="6"/>
@@ -5695,7 +5696,7 @@
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="6"/>
-      <c r="F175" s="6"/>
+      <c r="F175" s="14"/>
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
       <c r="I175" s="6"/>
@@ -5708,7 +5709,7 @@
       <c r="C176" s="3"/>
       <c r="D176" s="3"/>
       <c r="E176" s="6"/>
-      <c r="F176" s="6"/>
+      <c r="F176" s="14"/>
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
       <c r="I176" s="6"/>
@@ -5721,7 +5722,7 @@
       <c r="C177" s="3"/>
       <c r="D177" s="3"/>
       <c r="E177" s="6"/>
-      <c r="F177" s="6"/>
+      <c r="F177" s="14"/>
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
       <c r="I177" s="6"/>
@@ -5734,7 +5735,7 @@
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
       <c r="E178" s="6"/>
-      <c r="F178" s="6"/>
+      <c r="F178" s="14"/>
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
       <c r="I178" s="6"/>
@@ -5747,7 +5748,7 @@
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
       <c r="E179" s="6"/>
-      <c r="F179" s="6"/>
+      <c r="F179" s="14"/>
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
       <c r="I179" s="6"/>
@@ -5760,7 +5761,7 @@
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
       <c r="E180" s="6"/>
-      <c r="F180" s="6"/>
+      <c r="F180" s="14"/>
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
       <c r="I180" s="6"/>
@@ -5773,7 +5774,7 @@
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
       <c r="E181" s="6"/>
-      <c r="F181" s="6"/>
+      <c r="F181" s="14"/>
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
       <c r="I181" s="6"/>
@@ -5786,7 +5787,7 @@
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
       <c r="E182" s="6"/>
-      <c r="F182" s="6"/>
+      <c r="F182" s="14"/>
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
       <c r="I182" s="6"/>
@@ -5799,7 +5800,7 @@
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
       <c r="E183" s="6"/>
-      <c r="F183" s="6"/>
+      <c r="F183" s="14"/>
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
       <c r="I183" s="6"/>
@@ -5812,7 +5813,7 @@
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
       <c r="E184" s="6"/>
-      <c r="F184" s="6"/>
+      <c r="F184" s="14"/>
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
       <c r="I184" s="6"/>
@@ -5825,7 +5826,7 @@
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
       <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
+      <c r="F185" s="14"/>
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
       <c r="I185" s="6"/>
@@ -5838,7 +5839,7 @@
       <c r="C186" s="3"/>
       <c r="D186" s="3"/>
       <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
+      <c r="F186" s="14"/>
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
       <c r="I186" s="6"/>
@@ -5851,7 +5852,7 @@
       <c r="C187" s="3"/>
       <c r="D187" s="3"/>
       <c r="E187" s="6"/>
-      <c r="F187" s="6"/>
+      <c r="F187" s="14"/>
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
       <c r="I187" s="6"/>
@@ -5864,7 +5865,7 @@
       <c r="C188" s="3"/>
       <c r="D188" s="3"/>
       <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
+      <c r="F188" s="14"/>
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
       <c r="I188" s="6"/>
@@ -5877,7 +5878,7 @@
       <c r="C189" s="3"/>
       <c r="D189" s="3"/>
       <c r="E189" s="6"/>
-      <c r="F189" s="6"/>
+      <c r="F189" s="14"/>
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
       <c r="I189" s="6"/>
@@ -5890,7 +5891,7 @@
       <c r="C190" s="3"/>
       <c r="D190" s="3"/>
       <c r="E190" s="6"/>
-      <c r="F190" s="6"/>
+      <c r="F190" s="14"/>
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
       <c r="I190" s="6"/>
@@ -5903,7 +5904,7 @@
       <c r="C191" s="3"/>
       <c r="D191" s="3"/>
       <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
+      <c r="F191" s="14"/>
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
       <c r="I191" s="6"/>
@@ -5916,7 +5917,7 @@
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
       <c r="E192" s="6"/>
-      <c r="F192" s="6"/>
+      <c r="F192" s="14"/>
       <c r="G192" s="3"/>
       <c r="H192" s="3"/>
       <c r="I192" s="6"/>
@@ -5929,7 +5930,7 @@
       <c r="C193" s="3"/>
       <c r="D193" s="3"/>
       <c r="E193" s="6"/>
-      <c r="F193" s="6"/>
+      <c r="F193" s="14"/>
       <c r="G193" s="3"/>
       <c r="H193" s="3"/>
       <c r="I193" s="6"/>
@@ -5942,7 +5943,7 @@
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
       <c r="E194" s="6"/>
-      <c r="F194" s="6"/>
+      <c r="F194" s="14"/>
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
       <c r="I194" s="6"/>
@@ -5955,7 +5956,7 @@
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
       <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
+      <c r="F195" s="14"/>
       <c r="G195" s="3"/>
       <c r="H195" s="3"/>
       <c r="I195" s="6"/>
@@ -5968,7 +5969,7 @@
       <c r="C196" s="3"/>
       <c r="D196" s="3"/>
       <c r="E196" s="6"/>
-      <c r="F196" s="6"/>
+      <c r="F196" s="14"/>
       <c r="G196" s="3"/>
       <c r="H196" s="3"/>
       <c r="I196" s="6"/>
@@ -5981,7 +5982,7 @@
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
       <c r="E197" s="6"/>
-      <c r="F197" s="6"/>
+      <c r="F197" s="14"/>
       <c r="G197" s="3"/>
       <c r="H197" s="3"/>
       <c r="I197" s="6"/>
@@ -5994,7 +5995,7 @@
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
       <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
+      <c r="F198" s="14"/>
       <c r="G198" s="3"/>
       <c r="H198" s="3"/>
       <c r="I198" s="6"/>
@@ -6007,7 +6008,7 @@
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
       <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
+      <c r="F199" s="14"/>
       <c r="G199" s="3"/>
       <c r="H199" s="3"/>
       <c r="I199" s="6"/>
@@ -6020,7 +6021,7 @@
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
       <c r="E200" s="6"/>
-      <c r="F200" s="6"/>
+      <c r="F200" s="14"/>
       <c r="G200" s="3"/>
       <c r="H200" s="3"/>
       <c r="I200" s="6"/>
@@ -10793,7 +10794,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R250"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
write export to excel directly to template and include help
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/VERIFI-Import-Data.xlsx
+++ b/src/assets/csv_templates/VERIFI-Import-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak1\Dropbox (ORNL)\Armstrong Work\DOE VERIFI\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mroot\dev\VERIFI\src\assets\csv_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71FEF3C-D2BF-4B76-8166-B2FAB7BD64C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FFBF08-41DD-4E74-9E85-4C135CF4AA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="8" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2740,7 +2740,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -3271,299 +3271,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3585,428 +3292,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA44BA1C-33AA-438B-A66F-EC8668F3990F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609601" y="2095500"/>
-          <a:ext cx="12801600" cy="12449175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1"/>
-            <a:t>More Details</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> template is used both for setting up an initial data upload and for updating VERIFI each month, if you choose not to enter data manually within VERIFI. When uploading, you will be able to either replace your existing data (if you changed or updated some value entered previously) or ignore existing data and only upload what is new. When entering new data into the template, there is no need to sort by meter or date - VERIFI will use the meter number and date columns to separate and parse the data appropriately. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>This worksheet is password protected to protect the column names.  If you need to unlock it to modify the column widths or other things to better match your facility, the password is "VERIFI" but PLEASE do not change the column names (with the exception of the Predictors tab) as that will break VERIFI's ability to import data from this template.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>Facilities</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>First</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> start with the Facilities Tab, where you will setup the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>different facilities </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>in your company. Here the only required field is Facility Name, which used as a unique identifier for each set of data. This can be used to setup all your facilities and then the rest of the tabs left blank and you can use an alternative means of entering your meter setup and billing data. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>Meters-Utilities</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>Next you have the Meters-Utilities</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> Tab where you will setup the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>different metered inputs </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>into your facilities. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>You can add</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> an entry for each meter in your facilities, or rollup similar meters together. If you choose to add an entry for each incoming meter, VERIFI can help you merge them in the "Meter Grouping" section, so you can group all your electricity or other utilities together for analysis.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>Each column represents a data point to help VERIFI setup a meter:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>Facility Name </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>is used to assign meters to the different facilities. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>THIS IS REQUIRED.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>Meter Number</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is used as a unique identifier for each data stream, it can be your actual meter number or a self assigned name (not just numbers) to keep all your energy uses separate. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>THIS IS REQUIRED.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Source</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> represents the type of data being monitored: Electricity, Natural Gas, Other Fuels, Water, Wastewater, or other Utilities.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Phase and Fuel </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>are only used for "</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Other Fuels</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>" and help set the possible values for "Collection Unit".</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Collection Unit </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is the unit you are billed for (Natural Gas could be in MMBTU or in SCF)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Heat Capacity </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is the energy used for each unit of the collection unit (if the collection unit is not already an energy unit). VERIFI has some default values for this if you are unsure.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>Account Number, Meter</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t> Name, Utility Supplier, Notes, Building/Location </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>are all for your own note keeping / ease of use.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Meter Group </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>can be set in VERIFI and allows you to group multiple meters together for analysis.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Site-to-Source</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> is a factor used to convert site energy to source energy for Better Plants Reporting. </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>Most </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0"/>
-            <a:t>electricity it is usually estimated as 3, but on-site generated renewables (solar/wind) it is usually estimated as 1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>. For more details, please see the Better Plants Energy Baselining and Tracking Guidance Document. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Once this is setup, you should not need to enter data here again.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Meter Data Entry</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>When entering data, each row </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>represents a month for a single meter</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.  Including the meter number for each row allows you to enter data for all electricity meters on the same import file. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>You also do not have to "calendarize" your data before hand: if your meter is read in the middle of the month, VERIFI will help adjust your data to monthly data.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Electricity</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>The Electricity Tab is where you enter the data for your electricity meters.  Electricity is a separate entry because VERIFI allows you to track a lot more data for electricity (such as data relating to demand and other charges) to help you perform an Electricity Meter Analysis. Be sure to specify your facility name and the meter number for each data row</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Non-electricity</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>This tab is where you enter data for any other utility you wish to track, just be sure to have the facility name and correct meter number for each row.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Predictors</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>This tab is where you enter data pertaining to any predictors for correlation or regression analysis (weather data, production data, etc.).  On this tab, you can change the column names to match your facilities' preference (with the exception of "Date" and "Facility Name"). Be sure to have your facility name for each row.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -4139,123 +3424,109 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>277090</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>33975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B5D9A8-9DCD-C04F-BE97-155F451BD77B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1212272" y="2130136"/>
+          <a:ext cx="14218227" cy="13905839"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47776</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD28A103-51EA-49CA-818C-92481543DBC3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C529ACFE-B65E-3E26-F741-AB4C1DE7FA1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647825" y="952500"/>
-          <a:ext cx="12182475" cy="3428999"/>
+          <a:off x="3009900" y="1476375"/>
+          <a:ext cx="7772400" cy="2190901"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Facilities Help - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1"/>
-            <a:t>You can move or delete this text box</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
-            <a:t> as you enter data</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1800" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t>This page allows you to enter information about your facilities.  </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1800" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t>The only REQUIRED field here is the Facility Name. All the other data can be entered in VERIFI if you which, but it may be easier to get started here, especially if you have a lot of facilities.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1800" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t>This can be used to setup all your facilities and then the rest of the tabs left blank and you can use an alternative means of entering your meter setup and billing data. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1800" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t>You can copy and paste text, but should do so as "Paste as text"</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4263,437 +3534,54 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>156883</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>348599</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CABFE162-DDD1-4A82-8DF9-1606D8A78C20}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13EFD03-B168-13F1-BB55-E401397ECBC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="942975" y="762000"/>
-          <a:ext cx="14725650" cy="10062883"/>
+          <a:off x="2028825" y="1076325"/>
+          <a:ext cx="9978374" cy="6819900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Meters / Utilities Help - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1"/>
-            <a:t>You can move or delete this text box as you enter data</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>This </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>where you will setup the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>different metered inputs </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>into your facilities. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>To make setup faster - you can copy and paste any field's text, but should do so using "Paste as text" to perserve the formatting.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>In VERIFI a "Meter" is the general term used for a type</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> of utilities with a bill specifically for it and can include electricity, natural gas, water, other fuels, other energy sources, RECS, and more. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>You can add</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> an entry for each meter or bill in your facilities, or rollup similar entries together off sheet. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>If you choose to add an entry for each incoming meter, VERIFI can help you merge them in the "Meter Grouping" section or with the column "Meter Group". This allows you to group all your electricity or other utilities together for analysis, but still view them individually. You can even group all process electricity in one group and baseload electricity in another.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng"/>
-            <a:t>Most columns</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t> can be edited within VERIFI after data has been entered</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" u="sng"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>Each column represents a data point to help VERIFI setup a meter:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng"/>
-            <a:t>Facility Name </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>is used to assign meters to the different facilities. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>THIS IS REQUIRED.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng"/>
-            <a:t>Meter Number</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is used as a unique identifier for each data stream, it can be your actual meter number or a self assigned name (not just numbers) to keep all your energy uses separate. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>THIS IS REQUIRED AND MUST BE UNIQUE. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0"/>
-            <a:t>If you do not want to use meter numbers, then names like "Facility A - Electricity" are great.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Source</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> represents the type of data being monitored: Electricity, Natural Gas, Other Fuels, Water, Wastewater, or other Utilities. If you do not have an entry - then VERIFI will default to electricity. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Phase </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" u="none" baseline="0"/>
-            <a:t>and</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t> Fuel </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>are only used for "</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Other Fuels</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>" and help set the possible values for "Collection Unit".</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Collection Unit </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is the unit you are billed on (Natural Gas could be in MMBTU or in SCF). If you do not have an entry - the VERIFI will default to your facility's defaults from the settings page </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Heat Capacity </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is the energy used for each unit of the collection unit (if the collection unit is not already an energy unit). </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0"/>
-            <a:t>VERIFI has values for most fuels: if you are unsure you can leave this blank.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng"/>
-            <a:t>Account Number, Meter</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t> Name, Utility Supplier, Notes, Building/Location </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>are all for your own note keeping / ease of use.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Meter Group </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>can be set in VERIFI and allows you to group multiple meters together for analysis.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Site-to-Source</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> is a factor used to convert site energy to source energy for Better Plants Reporting. </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>Most </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0"/>
-            <a:t>electricity it is usually estimated as 3, but on-site generated renewables (solar/wind) it is usually estimated as 1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>. For more details, please see the Better Plants Energy Baselining and Tracking Guidance Document. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Calendarize Data? </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is used to designate if you want to have your data calendarized (bills reallocated to match calendar months) or not (designate July as "7-1-YYYY"). </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Scope</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t> is used to define the GHG Scope (Scope 1 vs Scope 2). VERIFI will assign values to this based on the Source for the meter.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Agreement Type </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is used only for Electricity - and will help set default values for Site-to-Source and the GHG emissions from the meter</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t>Include in Energy </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0"/>
-            <a:t>and</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Retain RECs </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>is used only for Electricity - and will help set default values for Site-to-Source and the GHG emissions from the meter and can be auto assigned based on Agreement type</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>Once this page is setup, you should not need to enter data here again unless you add facilities or meters.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4701,390 +3589,54 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>182410</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02DBFD2D-3FE5-4E58-885F-A940FEBE26F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB30291B-B559-A84F-19B9-E251FCE04203}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723900" y="952500"/>
-          <a:ext cx="14535150" cy="4572000"/>
+          <a:off x="1162050" y="1076324"/>
+          <a:ext cx="13517410" cy="4257675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Electricity Meter Data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-            <a:t> Entry </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Help - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1"/>
-            <a:t>You can move or delete this text box as you enter data</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>This </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>where you will enter </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-            <a:t>electricity bill data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>for your facilities. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>For VERIFI electricity meters also include self-generated electricity (solar/wind), PPPAs, VPPAs, RECS, etc.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>When entering data, each row </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>represents a single bill's electricity use for a single meter</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.  For most electricity bills, this would occur once a month, but for things like RECs, you might be billed quarterly  (see the Calendarization for more help with quarterly data).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>The </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Meter Number, Read Date, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>and</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Total Consumption </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>columns are all required</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Including the meter number for each row allows you to enter data for all electricity meters across all your facilities in the same import file. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Calendarization</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* You also do not have to "calendarize" your data before hand: if your meter is read in the middle of the month, VERIFI will help adjust your data to monthly data, just put in the meter read date.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* If your data is already calendarized - enter your date as the first of the month and select "No" for "Calendarize Data?" in the previous tab or select "Do not calendarize" within VERIFI upon upload.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* To enter quarterly bills, like for RECs, enter the bill date as the last day of the quarter. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>When getting started </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- to ensure your first year has a full 12 month - be sure to enter something for the month before you have actual data, even it if is a "bill" with a guessed date (or for quarterly the last day of the previous quarter) with a Total Consumption of 0. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Most of the columns in this tab are not required (everything after "Total Consumption") for upload and energy efficiency analyses. They are used for billing and cost analyses and demand analyses (which are not yet available in VERIFI). </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5092,407 +3644,54 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57256</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7536D981-9E4F-470C-92FA-8B6AF041F89C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EA7D0B0-7B73-4961-DB59-0818F5C7B080}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="942975" y="952500"/>
-          <a:ext cx="14630400" cy="4572000"/>
+          <a:off x="1781175" y="1524000"/>
+          <a:ext cx="12115906" cy="3790950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Non-Electricity Meter Data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-            <a:t> Entry </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Help - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1"/>
-            <a:t>You can move or delete this text box as you enter data</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>where you will enter </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>non-electricity bill data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>for your facilities including natural gas, other fuels (propane, coke oven gas), other energy sources (steam, compressed air), and other utilities (water, wastewater, refrigerant). </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>When entering data, each row </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>represents a single bill's utility use for a single meter</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.  For most electricity bills, this would occur once a month, but for some utilities, you might be billed quarterly (see the Calendarization for more help with quarterly data). </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>The </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Meter Number, Read Date, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>and</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Total Consumption </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>columns are all required</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Including the meter number for each row allows you to enter data for all additional meters across all your facilities in the same import file. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Calendarization</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* You also do not have to "calendarize" your data before hand: if your meter is read in the middle of the month, VERIFI will help adjust your data to monthly data, just put in the meter read date.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* If your data is already calendarized - enter your date as the first of the month and select "No" for "Calendarize Data?" in the previous tab or select "Do not calendarize" within VERIFI upon upload.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* To enter quarterly bills, like for RECs, enter the bill date as the last day of the quarter. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>* </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>When getting started </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- to ensure your first year has a full 12 month - be sure to enter something for the month before you have actual data, even it if is a "bill" with a guessed date (or for quarterly the last day of the previous quarter) with a Total Consumption of 0. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Most of the columns in this tab are not required (everything after "Total Consumption") for upload and energy efficiency analyses. They are used for billing and cost analyses and demand analyses (which are not yet available in VERIFI). </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5500,245 +3699,54 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>270533</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D4B6D4-62A3-4C95-B254-F4EFB952C24A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B553CF8-EDA9-9166-813A-B64957FDABAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647825" y="952500"/>
-          <a:ext cx="12134850" cy="4471147"/>
+          <a:off x="1962150" y="1114424"/>
+          <a:ext cx="9995558" cy="3686175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Predictor Data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-            <a:t> Entry </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>Help - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1"/>
-            <a:t>You can move or delete this text box as you enter data</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>where you will enter </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>data any quantifiable variable that could influence your energy use at</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> your facilities such as heating degree days, cooling degree days, production variables, humidity, average daily temperature, etc. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>When entering data, each row </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>represents a single month's predictors</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.  Enter dates as the first of the month. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>The </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Facility Name and Date</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>  are the only </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>columns required. Names for predictors are also required.  Each row does not have to an entry for a predictor.  If a predictor variable is only applicable to one facility, you can leave the value blank for any facility that does not use it and VERIFI will remove that predictor from the list for that facility. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6044,8 +4052,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B7:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6096,7 +4104,7 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8773,7 +6781,7 @@
   <dimension ref="A1:S201"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13566,8 +11574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7080E26A-D837-4A48-9A9A-3D27BF709F7E}">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13717,7 +11725,7 @@
         <v/>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C66" si="0">IF(B3="Electricity",A3,"")</f>
+        <f t="shared" ref="C3:C13" si="0">IF(B3="Electricity",A3,"")</f>
         <v/>
       </c>
       <c r="D3" t="str">
@@ -13746,7 +11754,7 @@
         <v/>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D67" si="1">IF(B4&lt;&gt;"Electricity",A4,"")</f>
+        <f t="shared" ref="D4:D13" si="1">IF(B4&lt;&gt;"Electricity",A4,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>